<commit_message>
Corrected chemicals with duplicate entries
</commit_message>
<xml_diff>
--- a/work/DallmanTable.xlsx
+++ b/work/DallmanTable.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACCE5FB2-C7DF-4874-9A76-B83ABB274369}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF60F6C-6B21-41F4-93F0-A868A6F6A4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="20265" windowHeight="11580" activeTab="1"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="27585" windowHeight="11490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DallmanTable" sheetId="1" r:id="rId1"/>
     <sheet name="TableforPaper" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="93">
   <si>
     <t>Drug</t>
   </si>
@@ -41,12 +52,6 @@
     <t>Dose</t>
   </si>
   <si>
-    <t>Dose.Units</t>
-  </si>
-  <si>
-    <t>Dosing.frequency</t>
-  </si>
-  <si>
     <t>Dose.Route</t>
   </si>
   <si>
@@ -68,49 +73,13 @@
     <t>Observed.Non.Pregnant</t>
   </si>
   <si>
-    <t>Predicted.Non.Pregnant</t>
-  </si>
-  <si>
-    <t>Ratio.Non.Pregnant</t>
-  </si>
-  <si>
     <t>Observed.Pregnant</t>
   </si>
   <si>
-    <t>Predicted.Pregnant</t>
-  </si>
-  <si>
-    <t>Ratio.Pregnant</t>
-  </si>
-  <si>
-    <t>Mass.Conversion</t>
-  </si>
-  <si>
-    <t>Converted.Units</t>
-  </si>
-  <si>
     <t>Observed.Non.Pregnant2</t>
   </si>
   <si>
-    <t>Predicted.Non.Pregnant3</t>
-  </si>
-  <si>
-    <t>Ratio.Non.Pregnant4</t>
-  </si>
-  <si>
     <t>Observed.Pregnant5</t>
-  </si>
-  <si>
-    <t>Predicted.Pregnant6</t>
-  </si>
-  <si>
-    <t>Ratio.Pregnant7</t>
-  </si>
-  <si>
-    <t>Source.observed.data.non.pregnant</t>
-  </si>
-  <si>
-    <t>Source.observed.data.pregnant</t>
   </si>
   <si>
     <t>Predicted.Non.Pregnant.httk</t>
@@ -274,11 +243,92 @@
   <si>
     <t>Predicted  Preg:Non Ratio</t>
   </si>
+  <si>
+    <t>Dose Units</t>
+  </si>
+  <si>
+    <t>Dosing frequency</t>
+  </si>
+  <si>
+    <t>Ratio Non-Pregnant</t>
+  </si>
+  <si>
+    <t>Ratio Pregnant</t>
+  </si>
+  <si>
+    <t>Mass Conversion</t>
+  </si>
+  <si>
+    <t>Converted Units</t>
+  </si>
+  <si>
+    <t>Predicted Non-Pregnant3</t>
+  </si>
+  <si>
+    <t>Ratio Non-Pregnant4</t>
+  </si>
+  <si>
+    <t>Predicted Pregnant6</t>
+  </si>
+  <si>
+    <t>Ratio Pregnant7</t>
+  </si>
+  <si>
+    <t>Source observed data non-pregnant</t>
+  </si>
+  <si>
+    <t>Source observed data pregnant</t>
+  </si>
+  <si>
+    <t>Diazepam</t>
+  </si>
+  <si>
+    <t>DTXSID4020406</t>
+  </si>
+  <si>
+    <t>439-14-5</t>
+  </si>
+  <si>
+    <t>AUClast</t>
+  </si>
+  <si>
+    <t>Metronidazole</t>
+  </si>
+  <si>
+    <t>DTXSID2020892</t>
+  </si>
+  <si>
+    <t>443-48-1</t>
+  </si>
+  <si>
+    <t>Digoxin</t>
+  </si>
+  <si>
+    <t>DTXSID5022934</t>
+  </si>
+  <si>
+    <t>20830-75-5</t>
+  </si>
+  <si>
+    <t>PMID: 18288078</t>
+  </si>
+  <si>
+    <t>Amoxicillin</t>
+  </si>
+  <si>
+    <t>DTXSID3037044</t>
+  </si>
+  <si>
+    <t>26787-78-0</t>
+  </si>
+  <si>
+    <t>PMID: 32748112</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1174,11 +1224,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AH9" sqref="A1:AH9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1243,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1203,102 +1253,102 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="X1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AA1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AF1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AG1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AH1" t="s">
         <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
       </c>
       <c r="E2">
         <v>194.19399999999999</v>
@@ -1307,13 +1357,13 @@
         <v>150</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="J2">
         <v>36</v>
@@ -1325,10 +1375,10 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="O2">
         <v>24.5</v>
@@ -1352,25 +1402,31 @@
         <v>1E-3</v>
       </c>
       <c r="V2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="W2">
-        <v>126.16</v>
+        <v>126.162497296518</v>
       </c>
       <c r="X2">
-        <v>145.22</v>
+        <v>145.21560913313499</v>
       </c>
       <c r="Y2">
-        <v>1.1499999999999999</v>
+        <v>1.15102040816327</v>
       </c>
       <c r="Z2">
-        <v>365.61</v>
+        <v>365.61376767562302</v>
       </c>
       <c r="AA2">
-        <v>312.57</v>
+        <v>312.57402391423</v>
       </c>
       <c r="AB2">
-        <v>0.85</v>
+        <v>0.85492957746478904</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>49</v>
       </c>
       <c r="AE2">
         <v>42.48</v>
@@ -1387,16 +1443,16 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
       </c>
       <c r="E3">
         <v>325.77</v>
@@ -1405,13 +1461,13 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="J3">
         <v>30</v>
@@ -1423,10 +1479,10 @@
         <v>0.25</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="O3">
         <v>17.899999999999999</v>
@@ -1450,28 +1506,34 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="W3">
-        <v>0.05</v>
+        <v>5.4946741566135597E-2</v>
       </c>
       <c r="X3">
-        <v>0.05</v>
+        <v>5.2491021272677102E-2</v>
       </c>
       <c r="Y3">
-        <v>0.96</v>
+        <v>0.955307262569833</v>
       </c>
       <c r="Z3">
-        <v>0.03</v>
+        <v>2.91616784848206E-2</v>
       </c>
       <c r="AA3">
-        <v>0.02</v>
+        <v>2.4188844890567E-2</v>
       </c>
       <c r="AB3">
-        <v>0.83</v>
+        <v>0.82947368421052603</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>49</v>
       </c>
       <c r="AE3">
-        <v>0.21057600000000001</v>
+        <v>0.21062400000000001</v>
       </c>
       <c r="AF3">
         <v>0.16308</v>
@@ -1480,21 +1542,21 @@
         <v>0.53072625698324005</v>
       </c>
       <c r="AH3">
-        <v>0.77444723045361297</v>
+        <v>0.77427073837739302</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
       </c>
       <c r="E4">
         <v>346.339</v>
@@ -1503,13 +1565,13 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="J4">
         <v>32</v>
@@ -1518,13 +1580,13 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.33</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="M4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="O4">
         <v>326</v>
@@ -1548,51 +1610,57 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="W4">
-        <v>0.94</v>
+        <v>0.94127430061298301</v>
       </c>
       <c r="X4">
-        <v>1.08</v>
+        <v>1.07697949119216</v>
       </c>
       <c r="Y4">
-        <v>1.1399999999999999</v>
+        <v>1.1441717791410999</v>
       </c>
       <c r="Z4">
-        <v>0.79</v>
+        <v>0.78535769867095495</v>
       </c>
       <c r="AA4">
-        <v>0.67</v>
+        <v>0.66697657497423002</v>
       </c>
       <c r="AB4">
-        <v>0.85</v>
+        <v>0.84926470588235303</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>49</v>
       </c>
       <c r="AE4">
         <v>3.0768</v>
       </c>
       <c r="AF4">
-        <v>1.7212799999999999</v>
+        <v>1.7296800000000001</v>
       </c>
       <c r="AG4">
         <v>0.83435582822085896</v>
       </c>
       <c r="AH4">
-        <v>0.55943837753510095</v>
+        <v>0.56216848673946995</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
       </c>
       <c r="E5">
         <v>267.36900000000003</v>
@@ -1601,13 +1669,13 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="J5">
         <v>37</v>
@@ -1619,10 +1687,10 @@
         <v>0.5</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="O5">
         <v>256</v>
@@ -1646,25 +1714,31 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V5" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="W5">
-        <v>0.96</v>
+        <v>0.95747824168097295</v>
       </c>
       <c r="X5">
-        <v>0.9</v>
+        <v>0.90137600095747805</v>
       </c>
       <c r="Y5">
-        <v>0.94</v>
+        <v>0.94140625</v>
       </c>
       <c r="Z5">
-        <v>0.45</v>
+        <v>0.45255807516952201</v>
       </c>
       <c r="AA5">
-        <v>0.49</v>
+        <v>0.49369971836675097</v>
       </c>
       <c r="AB5">
-        <v>1.0900000000000001</v>
+        <v>1.0909090909090899</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>49</v>
       </c>
       <c r="AE5">
         <v>0.66383999999999999</v>
@@ -1681,16 +1755,16 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
       </c>
       <c r="E6">
         <v>293.37</v>
@@ -1699,28 +1773,28 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="J6">
         <v>39</v>
       </c>
       <c r="K6">
-        <v>0.33</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="L6">
-        <v>0.33</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="M6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="O6">
         <v>234</v>
@@ -1744,51 +1818,57 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V6" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="W6">
-        <v>0.8</v>
+        <v>0.797627569281113</v>
       </c>
       <c r="X6">
-        <v>0.82</v>
+        <v>0.82489688788901405</v>
       </c>
       <c r="Y6">
-        <v>1.03</v>
+        <v>1.0341880341880301</v>
       </c>
       <c r="Z6">
-        <v>0.56000000000000005</v>
+        <v>0.55902103146197601</v>
       </c>
       <c r="AA6">
-        <v>0.54</v>
+        <v>0.53856904250604998</v>
       </c>
       <c r="AB6">
-        <v>0.96</v>
+        <v>0.96341463414634099</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>49</v>
       </c>
       <c r="AE6">
-        <v>0.6048</v>
+        <v>0.61031999999999997</v>
       </c>
       <c r="AF6">
-        <v>0.46776000000000001</v>
+        <v>0.47111999999999998</v>
       </c>
       <c r="AG6">
         <v>0.70085470085470103</v>
       </c>
       <c r="AH6">
-        <v>0.773412698412698</v>
+        <v>0.77192292567833298</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
       </c>
       <c r="E7">
         <v>312.41699999999997</v>
@@ -1797,13 +1877,13 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="J7">
         <v>15</v>
@@ -1815,10 +1895,10 @@
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N7" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="O7">
         <v>125</v>
@@ -1842,28 +1922,34 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="W7">
-        <v>0.4</v>
+        <v>0.40010626822484102</v>
       </c>
       <c r="X7">
-        <v>0.33</v>
+        <v>0.32968756501726898</v>
       </c>
       <c r="Y7">
-        <v>0.82</v>
+        <v>0.82399999999999995</v>
       </c>
       <c r="Z7">
-        <v>0.36</v>
+        <v>0.36169606647525598</v>
       </c>
       <c r="AA7">
-        <v>0.36</v>
+        <v>0.35529436618365801</v>
       </c>
       <c r="AB7">
-        <v>0.98</v>
+        <v>0.98230088495575196</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>49</v>
       </c>
       <c r="AE7">
-        <v>0.115536</v>
+        <v>0.115512</v>
       </c>
       <c r="AF7">
         <v>9.7367999999999996E-2</v>
@@ -1872,215 +1958,631 @@
         <v>0.90400000000000003</v>
       </c>
       <c r="AH7">
-        <v>0.84275031159119196</v>
+        <v>0.84292541034697699</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
       </c>
       <c r="E8">
-        <v>151.16300000000001</v>
+        <v>284.74</v>
       </c>
       <c r="F8">
-        <v>2000</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="J8">
-        <v>30.9</v>
+        <v>39</v>
       </c>
       <c r="K8">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="L8">
-        <v>0.25</v>
+        <v>0.41666666666666702</v>
       </c>
       <c r="M8" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="N8" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="O8">
-        <v>101.71</v>
-      </c>
-      <c r="P8" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>63</v>
+        <v>2.33</v>
+      </c>
+      <c r="P8">
+        <v>2.25</v>
+      </c>
+      <c r="Q8">
+        <v>0.96</v>
       </c>
       <c r="R8">
-        <v>74.3</v>
-      </c>
-      <c r="S8" t="s">
-        <v>63</v>
-      </c>
-      <c r="T8" t="s">
-        <v>63</v>
+        <v>0.7</v>
+      </c>
+      <c r="S8">
+        <v>0.63</v>
+      </c>
+      <c r="T8">
+        <v>0.9</v>
       </c>
       <c r="U8">
         <v>1E-3</v>
       </c>
       <c r="V8" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="W8">
-        <v>672.85</v>
-      </c>
-      <c r="X8" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>63</v>
+        <v>8.1829037016225303</v>
+      </c>
+      <c r="X8">
+        <v>7.9019456346140302</v>
+      </c>
+      <c r="Y8">
+        <v>0.96566523605150201</v>
       </c>
       <c r="Z8">
-        <v>491.52</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>63</v>
+        <v>2.4583830863243699</v>
+      </c>
+      <c r="AA8">
+        <v>2.2125447776919298</v>
+      </c>
+      <c r="AB8">
+        <v>0.9</v>
       </c>
       <c r="AC8" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="AD8" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="AE8">
-        <v>824.64</v>
+        <v>16.872</v>
       </c>
       <c r="AF8">
-        <v>551.28</v>
+        <v>4.6463999999999999</v>
       </c>
       <c r="AG8">
-        <v>0.73050830793432298</v>
+        <v>0.30042918454935602</v>
       </c>
       <c r="AH8">
-        <v>0.66850989522700799</v>
+        <v>0.27539118065433899</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
       </c>
       <c r="E9">
-        <v>321.2</v>
+        <v>171.15600000000001</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>500</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="I9" t="s">
         <v>39</v>
       </c>
       <c r="J9">
-        <v>38.4</v>
+        <v>39</v>
       </c>
       <c r="K9">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="L9">
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="N9" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="O9">
+        <v>151</v>
+      </c>
+      <c r="P9">
+        <v>170</v>
+      </c>
+      <c r="Q9">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="R9">
+        <v>102</v>
+      </c>
+      <c r="S9">
+        <v>112</v>
+      </c>
+      <c r="T9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U9">
+        <v>1E-3</v>
+      </c>
+      <c r="V9" t="s">
+        <v>28</v>
+      </c>
+      <c r="W9">
+        <v>882.23608871438898</v>
+      </c>
+      <c r="X9">
+        <v>993.24592769169601</v>
+      </c>
+      <c r="Y9">
+        <v>1.12582781456954</v>
+      </c>
+      <c r="Z9">
+        <v>595.94755661501802</v>
+      </c>
+      <c r="AA9">
+        <v>654.373787655706</v>
+      </c>
+      <c r="AB9">
+        <v>1.0980392156862699</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE9">
+        <v>102.98399999999999</v>
+      </c>
+      <c r="AF9">
+        <v>70.944000000000003</v>
+      </c>
+      <c r="AG9">
+        <v>0.67549668874172197</v>
+      </c>
+      <c r="AH9">
+        <v>0.688883710090888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10">
+        <v>151.16300000000001</v>
+      </c>
+      <c r="F10">
+        <v>2000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10">
+        <v>30.9</v>
+      </c>
+      <c r="K10">
+        <v>0.25</v>
+      </c>
+      <c r="L10">
+        <v>0.25</v>
+      </c>
+      <c r="M10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10">
+        <v>101.71</v>
+      </c>
+      <c r="P10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>49</v>
+      </c>
+      <c r="R10">
+        <v>74.3</v>
+      </c>
+      <c r="S10" t="s">
+        <v>49</v>
+      </c>
+      <c r="T10" t="s">
+        <v>49</v>
+      </c>
+      <c r="U10">
+        <v>1E-3</v>
+      </c>
+      <c r="V10" t="s">
+        <v>28</v>
+      </c>
+      <c r="W10">
+        <v>672.84983759253203</v>
+      </c>
+      <c r="X10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z10">
+        <v>491.52239635360502</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE10">
+        <v>824.88</v>
+      </c>
+      <c r="AF10">
+        <v>551.28</v>
+      </c>
+      <c r="AG10">
+        <v>0.73050830793432298</v>
+      </c>
+      <c r="AH10">
+        <v>0.66831539132964801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11">
+        <v>780.93799999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11">
+        <v>30.5</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>81</v>
+      </c>
+      <c r="N11" t="s">
+        <v>54</v>
+      </c>
+      <c r="O11">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="P11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>49</v>
+      </c>
+      <c r="R11">
+        <v>7.3</v>
+      </c>
+      <c r="S11" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" t="s">
+        <v>49</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W11">
+        <v>11.908755880748499</v>
+      </c>
+      <c r="X11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z11">
+        <v>9.3477331106950903</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE11">
+        <v>6.9503999999999996E-2</v>
+      </c>
+      <c r="AF11">
+        <v>4.1160000000000002E-2</v>
+      </c>
+      <c r="AG11">
+        <v>0.78494623655913998</v>
+      </c>
+      <c r="AH11">
+        <v>0.59219613259668502</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12">
+        <v>321.2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12">
+        <v>38.409999999999997</v>
+      </c>
+      <c r="K12">
+        <v>1.5</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" t="s">
+        <v>54</v>
+      </c>
+      <c r="O12">
         <v>560</v>
       </c>
-      <c r="P9" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>63</v>
-      </c>
-      <c r="R9">
+      <c r="P12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>49</v>
+      </c>
+      <c r="R12">
         <v>175.25</v>
       </c>
-      <c r="S9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T9" t="s">
-        <v>63</v>
-      </c>
-      <c r="U9">
+      <c r="S12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T12" t="s">
+        <v>49</v>
+      </c>
+      <c r="U12">
         <v>1</v>
       </c>
-      <c r="V9" t="s">
-        <v>42</v>
-      </c>
-      <c r="W9">
-        <v>1743.46</v>
-      </c>
-      <c r="X9" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z9">
-        <v>545.61</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE9">
+      <c r="V12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W12">
+        <v>1743.4620174346201</v>
+      </c>
+      <c r="X12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z12">
+        <v>545.61021170610195</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE12">
         <v>2.4384000000000001</v>
       </c>
-      <c r="AF9">
+      <c r="AF12">
         <v>1.82664</v>
       </c>
-      <c r="AG9">
+      <c r="AG12">
         <v>0.31294642857142901</v>
       </c>
-      <c r="AH9">
+      <c r="AH12">
         <v>0.74911417322834695</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13">
+        <v>365.4</v>
+      </c>
+      <c r="F13">
+        <v>2000</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13">
+        <v>35.1</v>
+      </c>
+      <c r="K13">
+        <v>0.25</v>
+      </c>
+      <c r="L13">
+        <v>0.1666667</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13">
+        <v>103.25278819280901</v>
+      </c>
+      <c r="P13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>49</v>
+      </c>
+      <c r="R13">
+        <v>87</v>
+      </c>
+      <c r="S13" t="s">
+        <v>49</v>
+      </c>
+      <c r="T13" t="s">
+        <v>49</v>
+      </c>
+      <c r="U13">
+        <v>1E-3</v>
+      </c>
+      <c r="V13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W13">
+        <v>282.57468033062099</v>
+      </c>
+      <c r="X13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z13">
+        <v>238.09523809523799</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE13">
+        <v>201.84</v>
+      </c>
+      <c r="AF13">
+        <v>119.688</v>
+      </c>
+      <c r="AG13">
+        <v>0.84259225850192598</v>
+      </c>
+      <c r="AH13">
+        <v>0.59298454221165298</v>
       </c>
     </row>
   </sheetData>
@@ -2090,11 +2592,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="A1:L9"/>
+      <selection activeCell="L13" sqref="A1:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,31 +2612,31 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2150,23 +2652,23 @@
         <f>DallmanTable!D2</f>
         <v>58-08-2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <f>DallmanTable!O2</f>
         <v>24.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <f>DallmanTable!R2</f>
         <v>71</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <f>DallmanTable!J2</f>
         <v>36</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <f>DallmanTable!K2</f>
         <v>0.5</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <f>DallmanTable!L2</f>
         <v>1</v>
       </c>
@@ -2200,29 +2702,29 @@
         <f>DallmanTable!D3</f>
         <v>59467-70-8</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <f>DallmanTable!O3</f>
         <v>17.899999999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <f>DallmanTable!R3</f>
         <v>9.5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <f>DallmanTable!J3</f>
         <v>30</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <f>DallmanTable!K3</f>
         <v>0.25</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <f>DallmanTable!L3</f>
         <v>0.25</v>
       </c>
       <c r="I3" s="4">
         <f>DallmanTable!AE3</f>
-        <v>0.21057600000000001</v>
+        <v>0.21062400000000001</v>
       </c>
       <c r="J3" s="4">
         <f>DallmanTable!AF3</f>
@@ -2234,7 +2736,7 @@
       </c>
       <c r="L3" s="4">
         <f>DallmanTable!AH3</f>
-        <v>0.77444723045361297</v>
+        <v>0.77427073837739302</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2250,25 +2752,25 @@
         <f>DallmanTable!D4</f>
         <v>21829-25-4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <f>DallmanTable!O4</f>
         <v>326</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <f>DallmanTable!R4</f>
         <v>272</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <f>DallmanTable!J4</f>
         <v>32</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <f>DallmanTable!K4</f>
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <f>DallmanTable!L4</f>
-        <v>0.33</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="I4" s="4">
         <f>DallmanTable!AE4</f>
@@ -2276,7 +2778,7 @@
       </c>
       <c r="J4" s="4">
         <f>DallmanTable!AF4</f>
-        <v>1.7212799999999999</v>
+        <v>1.7296800000000001</v>
       </c>
       <c r="K4" s="4">
         <f>DallmanTable!AG4</f>
@@ -2284,7 +2786,7 @@
       </c>
       <c r="L4" s="4">
         <f>DallmanTable!AH4</f>
-        <v>0.55943837753510095</v>
+        <v>0.56216848673946995</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2300,23 +2802,23 @@
         <f>DallmanTable!D5</f>
         <v>51384-51-1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <f>DallmanTable!O5</f>
         <v>256</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <f>DallmanTable!R5</f>
         <v>121</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <f>DallmanTable!J5</f>
         <v>37</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <f>DallmanTable!K5</f>
         <v>0.5</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <f>DallmanTable!L5</f>
         <v>0.5</v>
       </c>
@@ -2350,33 +2852,33 @@
         <f>DallmanTable!D6</f>
         <v>99614-02-5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <f>DallmanTable!O6</f>
         <v>234</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <f>DallmanTable!R6</f>
         <v>164</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <f>DallmanTable!J6</f>
         <v>39</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <f>DallmanTable!K6</f>
-        <v>0.33</v>
-      </c>
-      <c r="H6">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H6" s="4">
         <f>DallmanTable!L6</f>
-        <v>0.33</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="I6" s="4">
         <f>DallmanTable!AE6</f>
-        <v>0.6048</v>
+        <v>0.61031999999999997</v>
       </c>
       <c r="J6" s="4">
         <f>DallmanTable!AF6</f>
-        <v>0.46776000000000001</v>
+        <v>0.47111999999999998</v>
       </c>
       <c r="K6" s="4">
         <f>DallmanTable!AG6</f>
@@ -2384,7 +2886,7 @@
       </c>
       <c r="L6" s="4">
         <f>DallmanTable!AH6</f>
-        <v>0.773412698412698</v>
+        <v>0.77192292567833298</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2400,29 +2902,29 @@
         <f>DallmanTable!D7</f>
         <v>109889-09-0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <f>DallmanTable!O7</f>
         <v>125</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <f>DallmanTable!R7</f>
         <v>113</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <f>DallmanTable!J7</f>
         <v>15</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <f>DallmanTable!K7</f>
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <f>DallmanTable!L7</f>
         <v>1</v>
       </c>
       <c r="I7" s="4">
         <f>DallmanTable!AE7</f>
-        <v>0.115536</v>
+        <v>0.115512</v>
       </c>
       <c r="J7" s="4">
         <f>DallmanTable!AF7</f>
@@ -2434,116 +2936,316 @@
       </c>
       <c r="L7" s="4">
         <f>DallmanTable!AH7</f>
-        <v>0.84275031159119196</v>
+        <v>0.84292541034697699</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>DallmanTable!C8</f>
-        <v>Acetaminophen</v>
+        <v>Diazepam</v>
       </c>
       <c r="B8" t="str">
         <f>DallmanTable!B8</f>
-        <v>DTXSID2020006</v>
+        <v>DTXSID4020406</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>DallmanTable!D8</f>
-        <v>103-90-2</v>
-      </c>
-      <c r="D8">
+        <v>439-14-5</v>
+      </c>
+      <c r="D8" s="4">
         <f>DallmanTable!O8</f>
-        <v>101.71</v>
-      </c>
-      <c r="E8">
+        <v>2.33</v>
+      </c>
+      <c r="E8" s="4">
         <f>DallmanTable!R8</f>
-        <v>74.3</v>
-      </c>
-      <c r="F8">
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="4">
         <f>DallmanTable!J8</f>
-        <v>30.9</v>
-      </c>
-      <c r="G8">
+        <v>39</v>
+      </c>
+      <c r="G8" s="4">
         <f>DallmanTable!K8</f>
-        <v>0.25</v>
-      </c>
-      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
         <f>DallmanTable!L8</f>
-        <v>0.25</v>
+        <v>0.41666666666666702</v>
       </c>
       <c r="I8" s="4">
         <f>DallmanTable!AE8</f>
-        <v>824.64</v>
+        <v>16.872</v>
       </c>
       <c r="J8" s="4">
         <f>DallmanTable!AF8</f>
-        <v>551.28</v>
+        <v>4.6463999999999999</v>
       </c>
       <c r="K8" s="4">
         <f>DallmanTable!AG8</f>
-        <v>0.73050830793432298</v>
+        <v>0.30042918454935602</v>
       </c>
       <c r="L8" s="4">
         <f>DallmanTable!AH8</f>
-        <v>0.66850989522700799</v>
+        <v>0.27539118065433899</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>DallmanTable!C9</f>
-        <v>Lorazepam</v>
+        <v>Metronidazole</v>
       </c>
       <c r="B9" t="str">
         <f>DallmanTable!B9</f>
-        <v>DTXSID7023225</v>
+        <v>DTXSID2020892</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>DallmanTable!D9</f>
-        <v>846-49-1</v>
-      </c>
-      <c r="D9">
+        <v>443-48-1</v>
+      </c>
+      <c r="D9" s="4">
         <f>DallmanTable!O9</f>
-        <v>560</v>
-      </c>
-      <c r="E9">
+        <v>151</v>
+      </c>
+      <c r="E9" s="4">
         <f>DallmanTable!R9</f>
-        <v>175.25</v>
-      </c>
-      <c r="F9">
+        <v>102</v>
+      </c>
+      <c r="F9" s="4">
         <f>DallmanTable!J9</f>
-        <v>38.4</v>
-      </c>
-      <c r="G9">
+        <v>39</v>
+      </c>
+      <c r="G9" s="4">
         <f>DallmanTable!K9</f>
-        <v>1.5</v>
-      </c>
-      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4">
         <f>DallmanTable!L9</f>
         <v>2</v>
       </c>
       <c r="I9" s="4">
         <f>DallmanTable!AE9</f>
-        <v>2.4384000000000001</v>
+        <v>102.98399999999999</v>
       </c>
       <c r="J9" s="4">
         <f>DallmanTable!AF9</f>
-        <v>1.82664</v>
+        <v>70.944000000000003</v>
       </c>
       <c r="K9" s="4">
         <f>DallmanTable!AG9</f>
-        <v>0.31294642857142901</v>
+        <v>0.67549668874172197</v>
       </c>
       <c r="L9" s="4">
         <f>DallmanTable!AH9</f>
-        <v>0.74911417322834695</v>
+        <v>0.688883710090888</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="7" t="str">
+        <f>DallmanTable!C10</f>
+        <v>Acetaminophen</v>
+      </c>
+      <c r="B10" t="str">
+        <f>DallmanTable!B10</f>
+        <v>DTXSID2020006</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>DallmanTable!D10</f>
+        <v>103-90-2</v>
+      </c>
+      <c r="D10" s="4">
+        <f>DallmanTable!O10</f>
+        <v>101.71</v>
+      </c>
+      <c r="E10" s="4">
+        <f>DallmanTable!R10</f>
+        <v>74.3</v>
+      </c>
+      <c r="F10" s="4">
+        <f>DallmanTable!J10</f>
+        <v>30.9</v>
+      </c>
+      <c r="G10" s="4">
+        <f>DallmanTable!K10</f>
+        <v>0.25</v>
+      </c>
+      <c r="H10" s="4">
+        <f>DallmanTable!L10</f>
+        <v>0.25</v>
+      </c>
+      <c r="I10" s="4">
+        <f>DallmanTable!AE10</f>
+        <v>824.88</v>
+      </c>
+      <c r="J10" s="4">
+        <f>DallmanTable!AF10</f>
+        <v>551.28</v>
+      </c>
+      <c r="K10" s="4">
+        <f>DallmanTable!AG10</f>
+        <v>0.73050830793432298</v>
+      </c>
+      <c r="L10" s="4">
+        <f>DallmanTable!AH10</f>
+        <v>0.66831539132964801</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="7" t="str">
+        <f>DallmanTable!C11</f>
+        <v>Digoxin</v>
+      </c>
+      <c r="B11" t="str">
+        <f>DallmanTable!B11</f>
+        <v>DTXSID5022934</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>DallmanTable!D11</f>
+        <v>20830-75-5</v>
+      </c>
+      <c r="D11" s="4">
+        <f>DallmanTable!O11</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E11" s="4">
+        <f>DallmanTable!R11</f>
+        <v>7.3</v>
+      </c>
+      <c r="F11" s="4">
+        <f>DallmanTable!J11</f>
+        <v>30.5</v>
+      </c>
+      <c r="G11" s="4">
+        <f>DallmanTable!K11</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="4">
+        <f>DallmanTable!L11</f>
+        <v>2</v>
+      </c>
+      <c r="I11" s="4">
+        <f>DallmanTable!AE11</f>
+        <v>6.9503999999999996E-2</v>
+      </c>
+      <c r="J11" s="4">
+        <f>DallmanTable!AF11</f>
+        <v>4.1160000000000002E-2</v>
+      </c>
+      <c r="K11" s="4">
+        <f>DallmanTable!AG11</f>
+        <v>0.78494623655913998</v>
+      </c>
+      <c r="L11" s="4">
+        <f>DallmanTable!AH11</f>
+        <v>0.59219613259668502</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="str">
+        <f>DallmanTable!C12</f>
+        <v>Lorazepam</v>
+      </c>
+      <c r="B12" t="str">
+        <f>DallmanTable!B12</f>
+        <v>DTXSID7023225</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>DallmanTable!D12</f>
+        <v>846-49-1</v>
+      </c>
+      <c r="D12" s="4">
+        <f>DallmanTable!O12</f>
+        <v>560</v>
+      </c>
+      <c r="E12" s="4">
+        <f>DallmanTable!R12</f>
+        <v>175.25</v>
+      </c>
+      <c r="F12" s="4">
+        <f>DallmanTable!J12</f>
+        <v>38.409999999999997</v>
+      </c>
+      <c r="G12" s="4">
+        <f>DallmanTable!K12</f>
+        <v>1.5</v>
+      </c>
+      <c r="H12" s="4">
+        <f>DallmanTable!L12</f>
+        <v>2</v>
+      </c>
+      <c r="I12" s="4">
+        <f>DallmanTable!AE12</f>
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="J12" s="4">
+        <f>DallmanTable!AF12</f>
+        <v>1.82664</v>
+      </c>
+      <c r="K12" s="4">
+        <f>DallmanTable!AG12</f>
+        <v>0.31294642857142901</v>
+      </c>
+      <c r="L12" s="4">
+        <f>DallmanTable!AH12</f>
+        <v>0.74911417322834695</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="str">
+        <f>DallmanTable!C13</f>
+        <v>Amoxicillin</v>
+      </c>
+      <c r="B13" t="str">
+        <f>DallmanTable!B13</f>
+        <v>DTXSID3037044</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>DallmanTable!D13</f>
+        <v>26787-78-0</v>
+      </c>
+      <c r="D13" s="4">
+        <f>DallmanTable!O13</f>
+        <v>103.25278819280901</v>
+      </c>
+      <c r="E13" s="4">
+        <f>DallmanTable!R13</f>
+        <v>87</v>
+      </c>
+      <c r="F13" s="4">
+        <f>DallmanTable!J13</f>
+        <v>35.1</v>
+      </c>
+      <c r="G13" s="4">
+        <f>DallmanTable!K13</f>
+        <v>0.25</v>
+      </c>
+      <c r="H13" s="4">
+        <f>DallmanTable!L13</f>
+        <v>0.1666667</v>
+      </c>
+      <c r="I13" s="4">
+        <f>DallmanTable!AE13</f>
+        <v>201.84</v>
+      </c>
+      <c r="J13" s="4">
+        <f>DallmanTable!AF13</f>
+        <v>119.688</v>
+      </c>
+      <c r="K13" s="4">
+        <f>DallmanTable!AG13</f>
+        <v>0.84259225850192598</v>
+      </c>
+      <c r="L13" s="4">
+        <f>DallmanTable!AH13</f>
+        <v>0.59298454221165298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="C14" s="1"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>